<commit_message>
Added modified 723C to library
</commit_message>
<xml_diff>
--- a/Tandy/TRS-80/Tandy TRS-80 Color Computer 1/Documents/Tandy TRS-80 Color Computer 1 Bill of Materials.xlsx
+++ b/Tandy/TRS-80/Tandy TRS-80 Color Computer 1/Documents/Tandy TRS-80 Color Computer 1 Bill of Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Retro-Schematics\Tandy\TRS-80\Tandy TRS-80 Color Computer 1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5FF7E1-E55B-46A9-BE81-B856BF1C2C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D962B16-6704-489B-AF31-E3EE4ED5BC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36120" yWindow="-10520" windowWidth="28800" windowHeight="15560" tabRatio="635" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10840,7 +10840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3381E1D7-EDAC-4C5A-9BD3-14AA96894DD3}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>

</xml_diff>